<commit_message>
Mostly updated for the now (conditionally accepted) VEGF manuscript. -- LJS
</commit_message>
<xml_diff>
--- a/integrateAndSwitch/I&S comparison 090814.xlsx
+++ b/integrateAndSwitch/I&S comparison 090814.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="199">
   <si>
     <t>t=4mins</t>
   </si>
@@ -615,6 +615,12 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mode</t>
   </si>
 </sst>
 </file>
@@ -734,8 +740,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -787,9 +805,21 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6304,11 +6334,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125231672"/>
-        <c:axId val="2125234456"/>
+        <c:axId val="2103920792"/>
+        <c:axId val="2103917992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125231672"/>
+        <c:axId val="2103920792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6317,7 +6347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125234456"/>
+        <c:crossAx val="2103917992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6325,7 +6355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125234456"/>
+        <c:axId val="2103917992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6335,14 +6365,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125231672"/>
+        <c:crossAx val="2103920792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9311,10 +9340,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN44"/>
+  <dimension ref="A1:AN45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11011,6 +11040,30 @@
     </row>
     <row r="44" spans="1:20">
       <c r="A44" s="11"/>
+      <c r="R44" t="s">
+        <v>197</v>
+      </c>
+      <c r="S44">
+        <f>MEDIAN(S3:S40)</f>
+        <v>4</v>
+      </c>
+      <c r="T44">
+        <f>MEDIAN(T3:T40)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="R45" t="s">
+        <v>198</v>
+      </c>
+      <c r="S45">
+        <f>MODE(S3:S40)</f>
+        <v>4</v>
+      </c>
+      <c r="T45">
+        <f>MODE(T3:T40)</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:A112">

</xml_diff>